<commit_message>
operationId: IMPORT DC BILL LODGEMENT
</commit_message>
<xml_diff>
--- a/src/test/input/used/RSM/Deposit scope for_FSD_RSM_20250221.xlsx
+++ b/src/test/input/used/RSM/Deposit scope for_FSD_RSM_20250221.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28324"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28429"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Tata\CTBC Trade Finance\Letter of Credit\LC\Document for MVP4 FSD\RSM\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\eclipse_workspace\LC_GEN\src\test\input\group\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{14CDF8B3-F7A0-464B-81F2-D3897177126E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{267CEF3E-FAE0-4FB2-95CB-60EAEEE143B6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" firstSheet="1" activeTab="2" xr2:uid="{FD512113-F5B0-4DB7-82FF-ABFE321860E8}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="13900" firstSheet="1" activeTab="2" xr2:uid="{FD512113-F5B0-4DB7-82FF-ABFE321860E8}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" state="hidden" r:id="rId1"/>
@@ -859,7 +859,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="19">
+  <fonts count="19" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1378,7 +1378,7 @@
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="一般" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -1716,15 +1716,15 @@
       <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="3" max="3" width="14.28515625" customWidth="1"/>
-    <col min="4" max="4" width="43.42578125" customWidth="1"/>
-    <col min="6" max="6" width="11.140625" customWidth="1"/>
-    <col min="7" max="7" width="69.140625" customWidth="1"/>
+    <col min="3" max="3" width="14.296875" customWidth="1"/>
+    <col min="4" max="4" width="43.3984375" customWidth="1"/>
+    <col min="6" max="6" width="11.09765625" customWidth="1"/>
+    <col min="7" max="7" width="69.09765625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="25.5">
+    <row r="1" spans="1:8" ht="26" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1750,7 +1750,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:8">
+    <row r="2" spans="1:8" ht="15.5" x14ac:dyDescent="0.3">
       <c r="A2" s="4" t="s">
         <v>8</v>
       </c>
@@ -1776,7 +1776,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:8">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A3" s="12" t="s">
         <v>8</v>
       </c>
@@ -1802,7 +1802,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:8">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A4" s="4" t="s">
         <v>8</v>
       </c>
@@ -1828,7 +1828,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:8">
+    <row r="5" spans="1:8" ht="26" x14ac:dyDescent="0.3">
       <c r="A5" s="4" t="s">
         <v>8</v>
       </c>
@@ -1854,7 +1854,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="6" spans="1:8">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A6" s="4" t="s">
         <v>8</v>
       </c>
@@ -1880,7 +1880,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:8">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A7" s="12" t="s">
         <v>8</v>
       </c>
@@ -1906,7 +1906,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="8" spans="1:8">
+    <row r="8" spans="1:8" ht="26" x14ac:dyDescent="0.3">
       <c r="A8" s="4" t="s">
         <v>8</v>
       </c>
@@ -1932,7 +1932,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="9" spans="1:8">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A9" s="4" t="s">
         <v>8</v>
       </c>
@@ -1958,7 +1958,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="10" spans="1:8">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A10" s="4" t="s">
         <v>8</v>
       </c>
@@ -1984,7 +1984,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="11" spans="1:8">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A11" s="4" t="s">
         <v>8</v>
       </c>
@@ -2010,7 +2010,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="12" spans="1:8">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A12" s="7" t="s">
         <v>8</v>
       </c>
@@ -2036,7 +2036,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:8">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
       <c r="G15" s="15" t="s">
         <v>53</v>
       </c>
@@ -2058,21 +2058,21 @@
       <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="3" max="3" width="13.42578125" customWidth="1"/>
-    <col min="4" max="4" width="14.28515625" customWidth="1"/>
-    <col min="5" max="5" width="59.42578125" customWidth="1"/>
-    <col min="6" max="6" width="20.140625" customWidth="1"/>
+    <col min="3" max="3" width="13.3984375" customWidth="1"/>
+    <col min="4" max="4" width="14.296875" customWidth="1"/>
+    <col min="5" max="5" width="59.3984375" customWidth="1"/>
+    <col min="6" max="6" width="20.09765625" customWidth="1"/>
     <col min="7" max="7" width="10" customWidth="1"/>
-    <col min="8" max="8" width="33.7109375" customWidth="1"/>
-    <col min="9" max="9" width="22.85546875" customWidth="1"/>
-    <col min="10" max="10" width="15.7109375" customWidth="1"/>
-    <col min="11" max="11" width="24.140625" customWidth="1"/>
-    <col min="12" max="12" width="34.28515625" customWidth="1"/>
+    <col min="8" max="8" width="33.69921875" customWidth="1"/>
+    <col min="9" max="9" width="22.8984375" customWidth="1"/>
+    <col min="10" max="10" width="15.69921875" customWidth="1"/>
+    <col min="11" max="11" width="24.09765625" customWidth="1"/>
+    <col min="12" max="12" width="34.296875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="25.5">
+    <row r="1" spans="1:12" ht="26" x14ac:dyDescent="0.3">
       <c r="A1" s="38" t="s">
         <v>54</v>
       </c>
@@ -2110,7 +2110,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="2" spans="1:12">
+    <row r="2" spans="1:12" ht="25" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>1</v>
       </c>
@@ -2148,7 +2148,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="3" spans="1:12" ht="25.5">
+    <row r="3" spans="1:12" ht="25" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>2</v>
       </c>
@@ -2181,7 +2181,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="4" spans="1:12">
+    <row r="4" spans="1:12" ht="25" x14ac:dyDescent="0.3">
       <c r="B4" s="17" t="s">
         <v>79</v>
       </c>
@@ -2202,7 +2202,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="5" spans="1:12">
+    <row r="5" spans="1:12" ht="15" x14ac:dyDescent="0.35">
       <c r="A5">
         <v>3</v>
       </c>
@@ -2212,7 +2212,7 @@
       <c r="E5" s="20"/>
       <c r="F5" s="6"/>
     </row>
-    <row r="6" spans="1:12">
+    <row r="6" spans="1:12" ht="15" x14ac:dyDescent="0.35">
       <c r="A6">
         <v>4</v>
       </c>
@@ -2222,7 +2222,7 @@
       <c r="E6" s="20"/>
       <c r="F6" s="6"/>
     </row>
-    <row r="7" spans="1:12">
+    <row r="7" spans="1:12" ht="15" x14ac:dyDescent="0.35">
       <c r="A7">
         <v>5</v>
       </c>
@@ -2232,7 +2232,7 @@
       <c r="E7" s="20"/>
       <c r="F7" s="6"/>
     </row>
-    <row r="8" spans="1:12">
+    <row r="8" spans="1:12" ht="15" x14ac:dyDescent="0.35">
       <c r="A8">
         <v>6</v>
       </c>
@@ -2242,7 +2242,7 @@
       <c r="E8" s="20"/>
       <c r="F8" s="6"/>
     </row>
-    <row r="9" spans="1:12">
+    <row r="9" spans="1:12" ht="15.5" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>7</v>
       </c>
@@ -2253,7 +2253,7 @@
       <c r="F9" s="13"/>
       <c r="H9" s="16"/>
     </row>
-    <row r="10" spans="1:12">
+    <row r="10" spans="1:12" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A10">
         <v>8</v>
       </c>
@@ -2263,7 +2263,7 @@
       <c r="E10" s="20"/>
       <c r="F10" s="13"/>
     </row>
-    <row r="11" spans="1:12">
+    <row r="11" spans="1:12" ht="15" x14ac:dyDescent="0.35">
       <c r="A11">
         <v>9</v>
       </c>
@@ -2273,7 +2273,7 @@
       <c r="E11" s="20"/>
       <c r="F11" s="13"/>
     </row>
-    <row r="12" spans="1:12">
+    <row r="12" spans="1:12" ht="15" x14ac:dyDescent="0.35">
       <c r="A12">
         <v>10</v>
       </c>
@@ -2283,7 +2283,7 @@
       <c r="E12" s="20"/>
       <c r="F12" s="13"/>
     </row>
-    <row r="13" spans="1:12">
+    <row r="13" spans="1:12" ht="15" x14ac:dyDescent="0.35">
       <c r="A13">
         <v>11</v>
       </c>
@@ -2293,7 +2293,7 @@
       <c r="E13" s="20"/>
       <c r="F13" s="13"/>
     </row>
-    <row r="14" spans="1:12">
+    <row r="14" spans="1:12" ht="15" x14ac:dyDescent="0.35">
       <c r="A14">
         <v>12</v>
       </c>
@@ -2303,7 +2303,7 @@
       <c r="E14" s="20"/>
       <c r="F14" s="13"/>
     </row>
-    <row r="15" spans="1:12">
+    <row r="15" spans="1:12" ht="15.5" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>13</v>
       </c>
@@ -2314,7 +2314,7 @@
       <c r="F15" s="13"/>
       <c r="H15" s="16"/>
     </row>
-    <row r="16" spans="1:12">
+    <row r="16" spans="1:12" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A16">
         <v>14</v>
       </c>
@@ -2324,7 +2324,7 @@
       <c r="E16" s="25"/>
       <c r="F16" s="13"/>
     </row>
-    <row r="17" spans="1:8">
+    <row r="17" spans="1:8" ht="15" x14ac:dyDescent="0.35">
       <c r="A17">
         <v>15</v>
       </c>
@@ -2334,7 +2334,7 @@
       <c r="E17" s="31"/>
       <c r="F17" s="13"/>
     </row>
-    <row r="18" spans="1:8">
+    <row r="18" spans="1:8" ht="15" x14ac:dyDescent="0.35">
       <c r="A18">
         <v>16</v>
       </c>
@@ -2344,7 +2344,7 @@
       <c r="E18" s="31"/>
       <c r="F18" s="13"/>
     </row>
-    <row r="19" spans="1:8">
+    <row r="19" spans="1:8" ht="15" x14ac:dyDescent="0.35">
       <c r="A19">
         <v>17</v>
       </c>
@@ -2354,7 +2354,7 @@
       <c r="E19" s="31"/>
       <c r="F19" s="13"/>
     </row>
-    <row r="20" spans="1:8">
+    <row r="20" spans="1:8" ht="15" x14ac:dyDescent="0.35">
       <c r="A20">
         <v>18</v>
       </c>
@@ -2364,7 +2364,7 @@
       <c r="E20" s="31"/>
       <c r="F20" s="13"/>
     </row>
-    <row r="21" spans="1:8">
+    <row r="21" spans="1:8" ht="15" x14ac:dyDescent="0.35">
       <c r="A21">
         <v>19</v>
       </c>
@@ -2374,7 +2374,7 @@
       <c r="E21" s="31"/>
       <c r="F21" s="13"/>
     </row>
-    <row r="22" spans="1:8">
+    <row r="22" spans="1:8" ht="15" x14ac:dyDescent="0.35">
       <c r="A22">
         <v>20</v>
       </c>
@@ -2384,7 +2384,7 @@
       <c r="E22" s="31"/>
       <c r="F22" s="13"/>
     </row>
-    <row r="23" spans="1:8">
+    <row r="23" spans="1:8" ht="15" x14ac:dyDescent="0.35">
       <c r="A23">
         <v>21</v>
       </c>
@@ -2394,7 +2394,7 @@
       <c r="E23" s="20"/>
       <c r="F23" s="13"/>
     </row>
-    <row r="24" spans="1:8">
+    <row r="24" spans="1:8" ht="15" x14ac:dyDescent="0.35">
       <c r="A24">
         <v>22</v>
       </c>
@@ -2404,7 +2404,7 @@
       <c r="E24" s="20"/>
       <c r="F24" s="13"/>
     </row>
-    <row r="25" spans="1:8">
+    <row r="25" spans="1:8" ht="15" x14ac:dyDescent="0.35">
       <c r="A25">
         <v>23</v>
       </c>
@@ -2414,7 +2414,7 @@
       <c r="E25" s="20"/>
       <c r="F25" s="13"/>
     </row>
-    <row r="26" spans="1:8">
+    <row r="26" spans="1:8" ht="15.5" x14ac:dyDescent="0.3">
       <c r="A26">
         <v>24</v>
       </c>
@@ -2425,7 +2425,7 @@
       <c r="F26" s="6"/>
       <c r="H26" s="16"/>
     </row>
-    <row r="27" spans="1:8">
+    <row r="27" spans="1:8" ht="15" x14ac:dyDescent="0.35">
       <c r="A27">
         <v>25</v>
       </c>
@@ -2435,7 +2435,7 @@
       <c r="E27" s="20"/>
       <c r="F27" s="6"/>
     </row>
-    <row r="28" spans="1:8">
+    <row r="28" spans="1:8" ht="15" x14ac:dyDescent="0.35">
       <c r="A28">
         <v>26</v>
       </c>
@@ -2445,7 +2445,7 @@
       <c r="E28" s="20"/>
       <c r="F28" s="6"/>
     </row>
-    <row r="29" spans="1:8">
+    <row r="29" spans="1:8" ht="15" x14ac:dyDescent="0.35">
       <c r="A29">
         <v>27</v>
       </c>
@@ -2455,7 +2455,7 @@
       <c r="E29" s="20"/>
       <c r="F29" s="6"/>
     </row>
-    <row r="30" spans="1:8">
+    <row r="30" spans="1:8" ht="15" x14ac:dyDescent="0.35">
       <c r="A30">
         <v>28</v>
       </c>
@@ -2465,7 +2465,7 @@
       <c r="E30" s="20"/>
       <c r="F30" s="6"/>
     </row>
-    <row r="31" spans="1:8">
+    <row r="31" spans="1:8" ht="15" x14ac:dyDescent="0.35">
       <c r="A31">
         <v>29</v>
       </c>
@@ -2475,7 +2475,7 @@
       <c r="E31" s="20"/>
       <c r="F31" s="6"/>
     </row>
-    <row r="32" spans="1:8">
+    <row r="32" spans="1:8" ht="15" x14ac:dyDescent="0.35">
       <c r="A32">
         <v>30</v>
       </c>
@@ -2485,7 +2485,7 @@
       <c r="E32" s="20"/>
       <c r="F32" s="6"/>
     </row>
-    <row r="33" spans="1:8">
+    <row r="33" spans="1:8" ht="15" x14ac:dyDescent="0.35">
       <c r="A33">
         <v>31</v>
       </c>
@@ -2495,7 +2495,7 @@
       <c r="E33" s="20"/>
       <c r="F33" s="6"/>
     </row>
-    <row r="34" spans="1:8">
+    <row r="34" spans="1:8" ht="15.5" x14ac:dyDescent="0.3">
       <c r="A34">
         <v>32</v>
       </c>
@@ -2506,7 +2506,7 @@
       <c r="F34" s="6"/>
       <c r="H34" s="16"/>
     </row>
-    <row r="35" spans="1:8">
+    <row r="35" spans="1:8" ht="15.5" x14ac:dyDescent="0.3">
       <c r="A35">
         <v>33</v>
       </c>
@@ -2517,7 +2517,7 @@
       <c r="F35" s="13"/>
       <c r="H35" s="16"/>
     </row>
-    <row r="36" spans="1:8">
+    <row r="36" spans="1:8" ht="15.5" x14ac:dyDescent="0.3">
       <c r="A36">
         <v>34</v>
       </c>
@@ -2527,7 +2527,7 @@
       <c r="E36" s="33"/>
       <c r="F36" s="13"/>
     </row>
-    <row r="37" spans="1:8">
+    <row r="37" spans="1:8" ht="15.5" x14ac:dyDescent="0.3">
       <c r="A37">
         <v>35</v>
       </c>
@@ -2538,7 +2538,7 @@
       <c r="F37" s="6"/>
       <c r="H37" s="16"/>
     </row>
-    <row r="38" spans="1:8">
+    <row r="38" spans="1:8" ht="15" x14ac:dyDescent="0.35">
       <c r="A38">
         <v>36</v>
       </c>
@@ -2548,7 +2548,7 @@
       <c r="E38" s="20"/>
       <c r="F38" s="34"/>
     </row>
-    <row r="39" spans="1:8">
+    <row r="39" spans="1:8" ht="15" x14ac:dyDescent="0.35">
       <c r="A39">
         <v>37</v>
       </c>
@@ -2558,7 +2558,7 @@
       <c r="E39" s="20"/>
       <c r="F39" s="34"/>
     </row>
-    <row r="40" spans="1:8">
+    <row r="40" spans="1:8" ht="15" x14ac:dyDescent="0.35">
       <c r="A40">
         <v>38</v>
       </c>
@@ -2568,7 +2568,7 @@
       <c r="E40" s="20"/>
       <c r="F40" s="34"/>
     </row>
-    <row r="41" spans="1:8">
+    <row r="41" spans="1:8" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A41">
         <v>39</v>
       </c>
@@ -2578,7 +2578,7 @@
       <c r="E41" s="20"/>
       <c r="F41" s="34"/>
     </row>
-    <row r="42" spans="1:8">
+    <row r="42" spans="1:8" ht="15.5" x14ac:dyDescent="0.3">
       <c r="A42">
         <v>40</v>
       </c>
@@ -2589,7 +2589,7 @@
       <c r="F42" s="34"/>
       <c r="H42" s="16"/>
     </row>
-    <row r="43" spans="1:8">
+    <row r="43" spans="1:8" ht="15" x14ac:dyDescent="0.35">
       <c r="A43">
         <v>41</v>
       </c>
@@ -2599,7 +2599,7 @@
       <c r="E43" s="20"/>
       <c r="F43" s="34"/>
     </row>
-    <row r="44" spans="1:8">
+    <row r="44" spans="1:8" ht="15" x14ac:dyDescent="0.35">
       <c r="A44">
         <v>42</v>
       </c>
@@ -2609,7 +2609,7 @@
       <c r="E44" s="20"/>
       <c r="F44" s="34"/>
     </row>
-    <row r="45" spans="1:8">
+    <row r="45" spans="1:8" ht="15" x14ac:dyDescent="0.35">
       <c r="A45">
         <v>43</v>
       </c>
@@ -2619,7 +2619,7 @@
       <c r="E45" s="20"/>
       <c r="F45" s="34"/>
     </row>
-    <row r="46" spans="1:8">
+    <row r="46" spans="1:8" ht="15.5" x14ac:dyDescent="0.3">
       <c r="A46">
         <v>44</v>
       </c>
@@ -2630,7 +2630,7 @@
       <c r="F46" s="6"/>
       <c r="H46" s="16"/>
     </row>
-    <row r="47" spans="1:8">
+    <row r="47" spans="1:8" ht="15" x14ac:dyDescent="0.35">
       <c r="A47">
         <v>45</v>
       </c>
@@ -2640,7 +2640,7 @@
       <c r="E47" s="20"/>
       <c r="F47" s="6"/>
     </row>
-    <row r="48" spans="1:8">
+    <row r="48" spans="1:8" ht="15" x14ac:dyDescent="0.35">
       <c r="A48">
         <v>46</v>
       </c>
@@ -2650,7 +2650,7 @@
       <c r="E48" s="20"/>
       <c r="F48" s="6"/>
     </row>
-    <row r="49" spans="1:8">
+    <row r="49" spans="1:8" ht="15" x14ac:dyDescent="0.35">
       <c r="A49">
         <v>47</v>
       </c>
@@ -2660,7 +2660,7 @@
       <c r="E49" s="20"/>
       <c r="F49" s="6"/>
     </row>
-    <row r="50" spans="1:8">
+    <row r="50" spans="1:8" ht="15" x14ac:dyDescent="0.35">
       <c r="A50">
         <v>48</v>
       </c>
@@ -2670,7 +2670,7 @@
       <c r="E50" s="20"/>
       <c r="F50" s="6"/>
     </row>
-    <row r="51" spans="1:8">
+    <row r="51" spans="1:8" ht="15.5" x14ac:dyDescent="0.3">
       <c r="A51">
         <v>49</v>
       </c>
@@ -2681,7 +2681,7 @@
       <c r="F51" s="6"/>
       <c r="H51" s="16"/>
     </row>
-    <row r="52" spans="1:8">
+    <row r="52" spans="1:8" ht="15" x14ac:dyDescent="0.35">
       <c r="A52">
         <v>50</v>
       </c>
@@ -2691,7 +2691,7 @@
       <c r="E52" s="20"/>
       <c r="F52" s="6"/>
     </row>
-    <row r="53" spans="1:8">
+    <row r="53" spans="1:8" ht="15" x14ac:dyDescent="0.35">
       <c r="A53">
         <v>51</v>
       </c>
@@ -2701,7 +2701,7 @@
       <c r="E53" s="20"/>
       <c r="F53" s="6"/>
     </row>
-    <row r="54" spans="1:8">
+    <row r="54" spans="1:8" ht="15" x14ac:dyDescent="0.35">
       <c r="A54">
         <v>52</v>
       </c>
@@ -2711,7 +2711,7 @@
       <c r="E54" s="20"/>
       <c r="F54" s="6"/>
     </row>
-    <row r="55" spans="1:8">
+    <row r="55" spans="1:8" ht="15" x14ac:dyDescent="0.35">
       <c r="A55">
         <v>53</v>
       </c>
@@ -2721,7 +2721,7 @@
       <c r="E55" s="20"/>
       <c r="F55" s="6"/>
     </row>
-    <row r="56" spans="1:8">
+    <row r="56" spans="1:8" ht="15.5" x14ac:dyDescent="0.3">
       <c r="A56">
         <v>54</v>
       </c>
@@ -2732,10 +2732,10 @@
       <c r="F56" s="6"/>
       <c r="H56" s="16"/>
     </row>
-    <row r="57" spans="1:8">
+    <row r="57" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B57" s="41"/>
     </row>
-    <row r="58" spans="1:8">
+    <row r="58" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B58" s="41"/>
     </row>
   </sheetData>
@@ -2749,30 +2749,30 @@
   <dimension ref="A1:P81"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="F1" zoomScale="98" zoomScaleNormal="98" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A78" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G72" sqref="G72"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="J19" sqref="J19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15.75"/>
+  <sheetFormatPr defaultColWidth="9.09765625" defaultRowHeight="14.5" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="9.85546875" style="45" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.85546875" style="45" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.8984375" style="45" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.8984375" style="45" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="53" style="45" bestFit="1" customWidth="1"/>
-    <col min="4" max="5" width="28.140625" style="45" customWidth="1"/>
-    <col min="6" max="6" width="41.42578125" style="45" customWidth="1"/>
-    <col min="7" max="7" width="34.140625" style="56" customWidth="1"/>
-    <col min="8" max="8" width="14.28515625" style="45" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="11.5703125" style="45" customWidth="1"/>
-    <col min="10" max="10" width="18.28515625" style="45" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="49.28515625" style="45" customWidth="1"/>
-    <col min="12" max="12" width="22.7109375" style="45" customWidth="1"/>
+    <col min="4" max="5" width="28.09765625" style="45" customWidth="1"/>
+    <col min="6" max="6" width="41.3984375" style="45" customWidth="1"/>
+    <col min="7" max="7" width="34.09765625" style="56" customWidth="1"/>
+    <col min="8" max="8" width="14.296875" style="45" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11.59765625" style="45" customWidth="1"/>
+    <col min="10" max="10" width="18.296875" style="45" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="49.296875" style="45" customWidth="1"/>
+    <col min="12" max="12" width="22.69921875" style="45" customWidth="1"/>
     <col min="13" max="13" width="34" style="45" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="46.140625" style="45" customWidth="1"/>
-    <col min="15" max="15" width="44.28515625" style="45" customWidth="1"/>
-    <col min="16" max="16384" width="9.140625" style="45"/>
+    <col min="14" max="14" width="46.09765625" style="45" customWidth="1"/>
+    <col min="15" max="15" width="44.296875" style="45" customWidth="1"/>
+    <col min="16" max="16384" width="9.09765625" style="45"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A1" s="46" t="s">
         <v>129</v>
       </c>
@@ -2822,7 +2822,7 @@
         <v>233</v>
       </c>
     </row>
-    <row r="2" spans="1:16">
+    <row r="2" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A2" s="65" t="s">
         <v>130</v>
       </c>
@@ -2871,7 +2871,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:16">
+    <row r="3" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A3" s="65" t="s">
         <v>130</v>
       </c>
@@ -2922,7 +2922,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:16">
+    <row r="4" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A4" s="65" t="s">
         <v>130</v>
       </c>
@@ -2971,7 +2971,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:16">
+    <row r="5" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A5" s="65" t="s">
         <v>130</v>
       </c>
@@ -3022,7 +3022,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:16">
+    <row r="6" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A6" s="65" t="s">
         <v>130</v>
       </c>
@@ -3071,7 +3071,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:16">
+    <row r="7" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A7" s="65" t="s">
         <v>130</v>
       </c>
@@ -3122,7 +3122,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:16">
+    <row r="8" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A8" s="65" t="s">
         <v>130</v>
       </c>
@@ -3171,7 +3171,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:16">
+    <row r="9" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A9" s="65" t="s">
         <v>130</v>
       </c>
@@ -3222,7 +3222,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:16">
+    <row r="10" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A10" s="65" t="s">
         <v>130</v>
       </c>
@@ -3271,7 +3271,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:16">
+    <row r="11" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A11" s="65" t="s">
         <v>130</v>
       </c>
@@ -3320,7 +3320,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:16">
+    <row r="12" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A12" s="65" t="s">
         <v>130</v>
       </c>
@@ -3369,7 +3369,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:16">
+    <row r="13" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A13" s="65" t="s">
         <v>130</v>
       </c>
@@ -3418,7 +3418,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:16">
+    <row r="14" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A14" s="65" t="s">
         <v>130</v>
       </c>
@@ -3469,7 +3469,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:16">
+    <row r="15" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A15" s="65" t="s">
         <v>130</v>
       </c>
@@ -3518,7 +3518,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:16">
+    <row r="16" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A16" s="65" t="s">
         <v>130</v>
       </c>
@@ -3569,7 +3569,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:16">
+    <row r="17" spans="1:16" ht="15" x14ac:dyDescent="0.35">
       <c r="A17" s="65" t="s">
         <v>130</v>
       </c>
@@ -3618,7 +3618,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:16">
+    <row r="18" spans="1:16" ht="15" x14ac:dyDescent="0.35">
       <c r="A18" s="65" t="s">
         <v>130</v>
       </c>
@@ -3669,7 +3669,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:16">
+    <row r="19" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A19" s="65" t="s">
         <v>130</v>
       </c>
@@ -3698,7 +3698,7 @@
         <v>76</v>
       </c>
       <c r="J19" s="45" t="s">
-        <v>127</v>
+        <v>161</v>
       </c>
       <c r="K19" s="44" t="str">
         <f t="shared" si="0"/>
@@ -3718,7 +3718,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:16">
+    <row r="20" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A20" s="65" t="s">
         <v>130</v>
       </c>
@@ -3769,7 +3769,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:16">
+    <row r="21" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A21" s="65" t="s">
         <v>130</v>
       </c>
@@ -3818,7 +3818,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:16">
+    <row r="22" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A22" s="65" t="s">
         <v>130</v>
       </c>
@@ -3869,7 +3869,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:16">
+    <row r="23" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A23" s="65" t="s">
         <v>130</v>
       </c>
@@ -3918,7 +3918,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:16">
+    <row r="24" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A24" s="65" t="s">
         <v>130</v>
       </c>
@@ -3969,7 +3969,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:16">
+    <row r="25" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A25" s="65" t="s">
         <v>130</v>
       </c>
@@ -4018,7 +4018,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:16">
+    <row r="26" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A26" s="65" t="s">
         <v>130</v>
       </c>
@@ -4069,7 +4069,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:16">
+    <row r="27" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A27" s="65" t="s">
         <v>130</v>
       </c>
@@ -4117,7 +4117,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:16">
+    <row r="28" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A28" s="65" t="s">
         <v>130</v>
       </c>
@@ -4165,7 +4165,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:16">
+    <row r="29" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A29" s="65" t="s">
         <v>130</v>
       </c>
@@ -4213,7 +4213,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="1:16">
+    <row r="30" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A30" s="65" t="s">
         <v>130</v>
       </c>
@@ -4261,7 +4261,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:16">
+    <row r="31" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A31" s="65" t="s">
         <v>130</v>
       </c>
@@ -4309,7 +4309,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="1:16">
+    <row r="32" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A32" s="65" t="s">
         <v>130</v>
       </c>
@@ -4357,7 +4357,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="1:16">
+    <row r="33" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A33" s="65" t="s">
         <v>130</v>
       </c>
@@ -4408,7 +4408,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="1:16">
+    <row r="34" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A34" s="65" t="s">
         <v>130</v>
       </c>
@@ -4456,7 +4456,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="1:16">
+    <row r="35" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A35" s="65" t="s">
         <v>130</v>
       </c>
@@ -4504,7 +4504,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="1:16">
+    <row r="36" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A36" s="65" t="s">
         <v>130</v>
       </c>
@@ -4552,7 +4552,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="1:16">
+    <row r="37" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A37" s="65" t="s">
         <v>130</v>
       </c>
@@ -4600,7 +4600,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="38" spans="1:16">
+    <row r="38" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A38" s="65" t="s">
         <v>130</v>
       </c>
@@ -4648,7 +4648,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="39" spans="1:16">
+    <row r="39" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A39" s="65" t="s">
         <v>130</v>
       </c>
@@ -4696,7 +4696,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="40" spans="1:16">
+    <row r="40" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A40" s="65" t="s">
         <v>130</v>
       </c>
@@ -4744,7 +4744,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="41" spans="1:16">
+    <row r="41" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A41" s="65" t="s">
         <v>130</v>
       </c>
@@ -4792,7 +4792,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="42" spans="1:16">
+    <row r="42" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A42" s="65" t="s">
         <v>130</v>
       </c>
@@ -4840,7 +4840,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="43" spans="1:16">
+    <row r="43" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A43" s="65" t="s">
         <v>130</v>
       </c>
@@ -4888,7 +4888,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="44" spans="1:16">
+    <row r="44" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A44" s="65" t="s">
         <v>130</v>
       </c>
@@ -4936,7 +4936,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="45" spans="1:16">
+    <row r="45" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A45" s="65" t="s">
         <v>130</v>
       </c>
@@ -4984,7 +4984,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="46" spans="1:16">
+    <row r="46" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A46" s="65" t="s">
         <v>130</v>
       </c>
@@ -5032,7 +5032,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="47" spans="1:16">
+    <row r="47" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A47" s="45" t="s">
         <v>130</v>
       </c>
@@ -5080,7 +5080,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="48" spans="1:16">
+    <row r="48" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A48" s="65" t="s">
         <v>130</v>
       </c>
@@ -5131,7 +5131,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="49" spans="1:16">
+    <row r="49" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A49" s="65" t="s">
         <v>130</v>
       </c>
@@ -5179,7 +5179,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="50" spans="1:16">
+    <row r="50" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A50" s="65" t="s">
         <v>130</v>
       </c>
@@ -5227,7 +5227,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="51" spans="1:16">
+    <row r="51" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A51" s="65" t="s">
         <v>130</v>
       </c>
@@ -5275,7 +5275,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="52" spans="1:16">
+    <row r="52" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A52" s="65" t="s">
         <v>130</v>
       </c>
@@ -5323,7 +5323,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="53" spans="1:16">
+    <row r="53" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A53" s="65" t="s">
         <v>130</v>
       </c>
@@ -5371,7 +5371,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="54" spans="1:16">
+    <row r="54" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A54" s="65" t="s">
         <v>130</v>
       </c>
@@ -5419,7 +5419,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="55" spans="1:16">
+    <row r="55" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A55" s="65" t="s">
         <v>130</v>
       </c>
@@ -5467,7 +5467,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="56" spans="1:16">
+    <row r="56" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A56" s="65" t="s">
         <v>130</v>
       </c>
@@ -5515,7 +5515,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="57" spans="1:16">
+    <row r="57" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A57" s="65" t="s">
         <v>130</v>
       </c>
@@ -5563,7 +5563,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="58" spans="1:16">
+    <row r="58" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A58" s="65" t="s">
         <v>130</v>
       </c>
@@ -5611,7 +5611,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="59" spans="1:16">
+    <row r="59" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A59" s="65" t="s">
         <v>130</v>
       </c>
@@ -5659,7 +5659,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="60" spans="1:16">
+    <row r="60" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A60" s="65" t="s">
         <v>130</v>
       </c>
@@ -5707,7 +5707,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="61" spans="1:16">
+    <row r="61" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A61" s="65" t="s">
         <v>130</v>
       </c>
@@ -5755,7 +5755,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="62" spans="1:16">
+    <row r="62" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A62" s="45" t="s">
         <v>130</v>
       </c>
@@ -5803,7 +5803,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="63" spans="1:16">
+    <row r="63" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A63" s="65" t="s">
         <v>130</v>
       </c>
@@ -5854,7 +5854,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="64" spans="1:16">
+    <row r="64" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A64" s="65" t="s">
         <v>130</v>
       </c>
@@ -5902,7 +5902,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="65" spans="1:16">
+    <row r="65" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A65" s="65" t="s">
         <v>130</v>
       </c>
@@ -5950,7 +5950,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="66" spans="1:16">
+    <row r="66" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A66" s="65" t="s">
         <v>130</v>
       </c>
@@ -5998,7 +5998,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="67" spans="1:16">
+    <row r="67" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A67" s="65" t="s">
         <v>130</v>
       </c>
@@ -6046,7 +6046,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="68" spans="1:16">
+    <row r="68" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A68" s="65" t="s">
         <v>130</v>
       </c>
@@ -6094,7 +6094,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="69" spans="1:16">
+    <row r="69" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A69" s="65" t="s">
         <v>130</v>
       </c>
@@ -6142,7 +6142,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="70" spans="1:16">
+    <row r="70" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A70" s="65" t="s">
         <v>130</v>
       </c>
@@ -6190,7 +6190,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="71" spans="1:16">
+    <row r="71" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A71" s="65" t="s">
         <v>130</v>
       </c>
@@ -6238,7 +6238,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="72" spans="1:16">
+    <row r="72" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A72" s="65" t="s">
         <v>130</v>
       </c>
@@ -6286,7 +6286,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="73" spans="1:16">
+    <row r="73" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A73" s="65" t="s">
         <v>130</v>
       </c>
@@ -6334,7 +6334,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="74" spans="1:16">
+    <row r="74" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A74" s="65" t="s">
         <v>130</v>
       </c>
@@ -6382,7 +6382,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="75" spans="1:16">
+    <row r="75" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A75" s="65" t="s">
         <v>130</v>
       </c>
@@ -6430,7 +6430,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="76" spans="1:16">
+    <row r="76" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A76" s="65" t="s">
         <v>130</v>
       </c>
@@ -6478,7 +6478,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="77" spans="1:16">
+    <row r="77" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A77" s="45" t="s">
         <v>130</v>
       </c>
@@ -6526,7 +6526,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="78" spans="1:16">
+    <row r="78" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A78" s="45" t="s">
         <v>130</v>
       </c>
@@ -6574,7 +6574,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="79" spans="1:16">
+    <row r="79" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A79" s="45" t="s">
         <v>130</v>
       </c>
@@ -6622,7 +6622,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="80" spans="1:16">
+    <row r="80" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A80" s="45" t="s">
         <v>130</v>
       </c>
@@ -6670,7 +6670,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="81" spans="1:16">
+    <row r="81" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A81" s="45" t="s">
         <v>130</v>
       </c>
@@ -6733,14 +6733,14 @@
       <selection activeCell="B67" sqref="B67"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="8.5703125" style="45" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="255.7109375" style="45" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="70.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="8.59765625" style="45" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="255.69921875" style="45" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="70.59765625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" s="46" t="s">
         <v>90</v>
       </c>
@@ -6748,7 +6748,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="2" spans="1:3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" s="45" t="s">
         <v>142</v>
       </c>
@@ -6760,7 +6760,7 @@
         <v>PATCH /v2/inventory/{inventory-lot-reference}/{instrument-ref}/leaf-status</v>
       </c>
     </row>
-    <row r="3" spans="1:3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" s="45" t="s">
         <v>142</v>
       </c>
@@ -6772,7 +6772,7 @@
         <v>PATCH /v2/inventory/{inventory-lot-reference}/{instrument-ref}/leaf-status</v>
       </c>
     </row>
-    <row r="4" spans="1:3">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" s="45" t="s">
         <v>142</v>
       </c>
@@ -6784,7 +6784,7 @@
         <v>PATCH /v2/inventory/{inventory-lot-reference}/{instrument-ref}/leaf-status</v>
       </c>
     </row>
-    <row r="5" spans="1:3">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" s="45" t="s">
         <v>142</v>
       </c>
@@ -6796,7 +6796,7 @@
         <v>PATCH /v2/inventory/{inventory-lot-reference}/{instrument-ref}/leaf-status</v>
       </c>
     </row>
-    <row r="6" spans="1:3">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" s="45" t="s">
         <v>143</v>
       </c>
@@ -6808,7 +6808,7 @@
         <v>GET /v2/inventory/{instrument-type}?teller=&lt;String&gt;&amp;instrument-type=&lt;Numeric&gt;&amp;inventory-lot-ref=&lt;String&gt;&amp;currency=&lt;String&gt;&amp;inventory-status=&lt;Numeric&gt;&amp;inventory-type=&lt;Numeric&gt;&amp;page-num=&lt;Numeric&gt;&amp;page-size=&lt;Numeric&gt;</v>
       </c>
     </row>
-    <row r="7" spans="1:3">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" s="45" t="s">
         <v>143</v>
       </c>
@@ -6820,7 +6820,7 @@
         <v>GET /v2/inventory/{instrument-type}?teller=&lt;String&gt;&amp;instrument-type=&lt;Numeric&gt;&amp;inventory-lot-ref=&lt;String&gt;&amp;currency=&lt;String&gt;&amp;inventory-status=&lt;Numeric&gt;&amp;inventory-type=&lt;Numeric&gt;&amp;page-num=&lt;Numeric&gt;&amp;page-size=&lt;Numeric&gt;</v>
       </c>
     </row>
-    <row r="8" spans="1:3">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8" s="45" t="s">
         <v>91</v>
       </c>
@@ -6832,7 +6832,7 @@
         <v>POST /v2/inventory/inventory-transfer</v>
       </c>
     </row>
-    <row r="9" spans="1:3">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9" s="45" t="s">
         <v>91</v>
       </c>
@@ -6844,7 +6844,7 @@
         <v>POST /v2/inventory/inventory-transfer</v>
       </c>
     </row>
-    <row r="10" spans="1:3">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A10" s="45" t="s">
         <v>91</v>
       </c>
@@ -6856,7 +6856,7 @@
         <v>POST /v2/inventory/inventory-transfer</v>
       </c>
     </row>
-    <row r="11" spans="1:3">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A11" s="45" t="s">
         <v>91</v>
       </c>
@@ -6868,7 +6868,7 @@
         <v>POST /v2/inventory/inventory-transfer</v>
       </c>
     </row>
-    <row r="12" spans="1:3">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A12" s="45" t="s">
         <v>91</v>
       </c>
@@ -6880,7 +6880,7 @@
         <v>POST /v2/inventory/inventory-transfer</v>
       </c>
     </row>
-    <row r="13" spans="1:3">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A13" s="45" t="s">
         <v>143</v>
       </c>
@@ -6892,7 +6892,7 @@
         <v>GET /v2/inventory/{instrument-type}/inventory-transfer-list?transfer-request-type=&lt;Numeric&gt;&amp;from-teller=&lt;String&gt;&amp;to-teller=&lt;String&gt;&amp;transfer-date=&lt;Date&gt;&amp;inventory-lot-reference=&lt;String&gt;&amp;transfer-order-status=&lt;Numeric&gt;&amp;inventory-currency=&lt;String&gt;&amp;page-num=&lt;Numeric&gt;&amp;page-size=&lt;Numeric&gt;</v>
       </c>
     </row>
-    <row r="14" spans="1:3">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A14" s="45" t="s">
         <v>143</v>
       </c>
@@ -6904,7 +6904,7 @@
         <v>GET /v2/inventory/{instrument-type}/inventory-transfer-list?transfer-request-type=&lt;Numeric&gt;&amp;from-teller=&lt;String&gt;&amp;to-teller=&lt;String&gt;&amp;transfer-date=&lt;Date&gt;&amp;inventory-lot-reference=&lt;String&gt;&amp;transfer-order-status=&lt;Numeric&gt;&amp;inventory-currency=&lt;String&gt;&amp;page-num=&lt;Numeric&gt;&amp;page-size=&lt;Numeric&gt;</v>
       </c>
     </row>
-    <row r="15" spans="1:3">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A15" s="45" t="s">
         <v>143</v>
       </c>
@@ -6916,7 +6916,7 @@
         <v>GET /v2/inventory/{instrument-type}/inventory-lot?instrument-status=&lt;Numeric&gt;&amp;start-serial-no=&lt;Numeric&gt;&amp;end-serial-no=&lt;Numeric&gt;&amp;page-num=&lt;Numeric&gt;&amp;page-size=&lt;Numeric&gt;</v>
       </c>
     </row>
-    <row r="16" spans="1:3">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A16" s="45" t="s">
         <v>143</v>
       </c>
@@ -6928,7 +6928,7 @@
         <v>GET /v2/inventory/{instrument-type}/inventory-lot?instrument-status=&lt;Numeric&gt;&amp;start-serial-no=&lt;Numeric&gt;&amp;end-serial-no=&lt;Numeric&gt;&amp;page-num=&lt;Numeric&gt;&amp;page-size=&lt;Numeric&gt;</v>
       </c>
     </row>
-    <row r="17" spans="1:3">
+    <row r="17" spans="1:3" ht="15" x14ac:dyDescent="0.35">
       <c r="A17" s="45" t="s">
         <v>91</v>
       </c>
@@ -6940,7 +6940,7 @@
         <v>POST /v2/inventory</v>
       </c>
     </row>
-    <row r="18" spans="1:3">
+    <row r="18" spans="1:3" ht="15" x14ac:dyDescent="0.35">
       <c r="A18" s="45" t="s">
         <v>91</v>
       </c>
@@ -6952,7 +6952,7 @@
         <v>POST /v2/inventory</v>
       </c>
     </row>
-    <row r="19" spans="1:3">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A19" s="45" t="s">
         <v>143</v>
       </c>
@@ -6964,7 +6964,7 @@
         <v>GET /v2/inventory/{instrument-type}/{inventory-lot-ref}/inventory-lot-details</v>
       </c>
     </row>
-    <row r="20" spans="1:3">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A20" s="45" t="s">
         <v>143</v>
       </c>
@@ -6976,7 +6976,7 @@
         <v>GET /v2/inventory/{instrument-type}/{inventory-lot-ref}/inventory-lot-details</v>
       </c>
     </row>
-    <row r="21" spans="1:3">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A21" s="45" t="s">
         <v>142</v>
       </c>
@@ -6988,7 +6988,7 @@
         <v>PATCH /v2/inventory/{instrument-type}/{inventory-lot-ref}/{requesting-user-id}</v>
       </c>
     </row>
-    <row r="22" spans="1:3">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A22" s="45" t="s">
         <v>142</v>
       </c>
@@ -7000,7 +7000,7 @@
         <v>PATCH /v2/inventory/{instrument-type}/{inventory-lot-ref}/{requesting-user-id}</v>
       </c>
     </row>
-    <row r="23" spans="1:3">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A23" s="45" t="s">
         <v>142</v>
       </c>
@@ -7012,7 +7012,7 @@
         <v>PATCH /v2/inventory/{instrument-type}/{inventory-lot-ref}/{requesting-user-id}</v>
       </c>
     </row>
-    <row r="24" spans="1:3">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A24" s="45" t="s">
         <v>142</v>
       </c>
@@ -7024,7 +7024,7 @@
         <v>PATCH /v2/inventory/{instrument-type}/{inventory-lot-ref}/{requesting-user-id}</v>
       </c>
     </row>
-    <row r="25" spans="1:3">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A25" s="45" t="s">
         <v>143</v>
       </c>
@@ -7036,7 +7036,7 @@
         <v>GET /v2/inventory/{instrument-type}/{inventory-lot-ref}</v>
       </c>
     </row>
-    <row r="26" spans="1:3">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A26" s="45" t="s">
         <v>143</v>
       </c>
@@ -7048,7 +7048,7 @@
         <v>GET /v2/inventory/{instrument-type}/{inventory-lot-ref}</v>
       </c>
     </row>
-    <row r="27" spans="1:3">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A27" s="45" t="s">
         <v>143</v>
       </c>
@@ -7060,7 +7060,7 @@
         <v>GET /v2/inventory/{instrument-type}/{inventory-lot-ref}</v>
       </c>
     </row>
-    <row r="28" spans="1:3">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A28" s="45" t="s">
         <v>143</v>
       </c>
@@ -7072,7 +7072,7 @@
         <v>GET /v2/inventory/{instrument-type}/{inventory-lot-ref}</v>
       </c>
     </row>
-    <row r="29" spans="1:3">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A29" s="45" t="s">
         <v>143</v>
       </c>
@@ -7084,7 +7084,7 @@
         <v>GET /v2/inventory/{instrument-type}/{inventory-lot-ref}</v>
       </c>
     </row>
-    <row r="30" spans="1:3">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A30" s="45" t="s">
         <v>143</v>
       </c>
@@ -7096,7 +7096,7 @@
         <v>GET /v2/inventory/{instrument-type}/{inventory-lot-ref}</v>
       </c>
     </row>
-    <row r="31" spans="1:3">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A31" s="45" t="s">
         <v>143</v>
       </c>
@@ -7108,7 +7108,7 @@
         <v>GET /v2/inventory/{instrument-type}/{inventory-lot-ref}</v>
       </c>
     </row>
-    <row r="32" spans="1:3">
+    <row r="32" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A32" s="45" t="s">
         <v>143</v>
       </c>
@@ -7120,7 +7120,7 @@
         <v>GET /v2/inventory/{instrument-type}/{inventory-lot-ref}</v>
       </c>
     </row>
-    <row r="33" spans="1:3">
+    <row r="33" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A33" s="45" t="s">
         <v>91</v>
       </c>
@@ -7132,7 +7132,7 @@
         <v>POST /v2/travelers-cheque-purchase</v>
       </c>
     </row>
-    <row r="34" spans="1:3">
+    <row r="34" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A34" s="45" t="s">
         <v>91</v>
       </c>
@@ -7144,7 +7144,7 @@
         <v>POST /v2/travelers-cheque-purchase</v>
       </c>
     </row>
-    <row r="35" spans="1:3">
+    <row r="35" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A35" s="45" t="s">
         <v>91</v>
       </c>
@@ -7156,7 +7156,7 @@
         <v>POST /v2/travelers-cheque-purchase</v>
       </c>
     </row>
-    <row r="36" spans="1:3">
+    <row r="36" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A36" s="45" t="s">
         <v>91</v>
       </c>
@@ -7168,7 +7168,7 @@
         <v>POST /v2/travelers-cheque-purchase</v>
       </c>
     </row>
-    <row r="37" spans="1:3">
+    <row r="37" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A37" s="45" t="s">
         <v>91</v>
       </c>
@@ -7180,7 +7180,7 @@
         <v>POST /v2/travelers-cheque-purchase</v>
       </c>
     </row>
-    <row r="38" spans="1:3">
+    <row r="38" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A38" s="45" t="s">
         <v>91</v>
       </c>
@@ -7192,7 +7192,7 @@
         <v>POST /v2/travelers-cheque-purchase</v>
       </c>
     </row>
-    <row r="39" spans="1:3">
+    <row r="39" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A39" s="45" t="s">
         <v>91</v>
       </c>
@@ -7204,7 +7204,7 @@
         <v>POST /v2/travelers-cheque-purchase</v>
       </c>
     </row>
-    <row r="40" spans="1:3">
+    <row r="40" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A40" s="45" t="s">
         <v>91</v>
       </c>
@@ -7216,7 +7216,7 @@
         <v>POST /v2/travelers-cheque-purchase</v>
       </c>
     </row>
-    <row r="41" spans="1:3">
+    <row r="41" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A41" s="45" t="s">
         <v>91</v>
       </c>
@@ -7228,7 +7228,7 @@
         <v>POST /v2/travelers-cheque-purchase</v>
       </c>
     </row>
-    <row r="42" spans="1:3">
+    <row r="42" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A42" s="45" t="s">
         <v>91</v>
       </c>
@@ -7240,7 +7240,7 @@
         <v>POST /v2/travelers-cheque-purchase</v>
       </c>
     </row>
-    <row r="43" spans="1:3">
+    <row r="43" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A43" s="45" t="s">
         <v>91</v>
       </c>
@@ -7252,7 +7252,7 @@
         <v>POST /v2/travelers-cheque-purchase</v>
       </c>
     </row>
-    <row r="44" spans="1:3">
+    <row r="44" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A44" s="45" t="s">
         <v>91</v>
       </c>
@@ -7264,7 +7264,7 @@
         <v>POST /v2/travelers-cheque-purchase</v>
       </c>
     </row>
-    <row r="45" spans="1:3">
+    <row r="45" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A45" s="45" t="s">
         <v>91</v>
       </c>
@@ -7276,7 +7276,7 @@
         <v>POST /v2/travelers-cheque-purchase</v>
       </c>
     </row>
-    <row r="46" spans="1:3">
+    <row r="46" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A46" s="45" t="s">
         <v>91</v>
       </c>
@@ -7288,7 +7288,7 @@
         <v>POST /v2/travelers-cheque-purchase</v>
       </c>
     </row>
-    <row r="47" spans="1:3">
+    <row r="47" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A47" s="45" t="s">
         <v>91</v>
       </c>
@@ -7300,7 +7300,7 @@
         <v>POST /v2/travelers-cheque-purchase</v>
       </c>
     </row>
-    <row r="48" spans="1:3">
+    <row r="48" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A48" s="45" t="s">
         <v>204</v>
       </c>
@@ -7312,7 +7312,7 @@
         <v>PUT /v2/travelers-cheque-purchase/{tcheque-purchase-reference}</v>
       </c>
     </row>
-    <row r="49" spans="1:3">
+    <row r="49" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A49" s="45" t="s">
         <v>204</v>
       </c>
@@ -7324,7 +7324,7 @@
         <v>PUT /v2/travelers-cheque-purchase/{tcheque-purchase-reference}</v>
       </c>
     </row>
-    <row r="50" spans="1:3">
+    <row r="50" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A50" s="45" t="s">
         <v>204</v>
       </c>
@@ -7336,7 +7336,7 @@
         <v>PUT /v2/travelers-cheque-purchase/{tcheque-purchase-reference}</v>
       </c>
     </row>
-    <row r="51" spans="1:3">
+    <row r="51" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A51" s="45" t="s">
         <v>204</v>
       </c>
@@ -7348,7 +7348,7 @@
         <v>PUT /v2/travelers-cheque-purchase/{tcheque-purchase-reference}</v>
       </c>
     </row>
-    <row r="52" spans="1:3">
+    <row r="52" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A52" s="45" t="s">
         <v>204</v>
       </c>
@@ -7360,7 +7360,7 @@
         <v>PUT /v2/travelers-cheque-purchase/{tcheque-purchase-reference}</v>
       </c>
     </row>
-    <row r="53" spans="1:3">
+    <row r="53" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A53" s="45" t="s">
         <v>204</v>
       </c>
@@ -7372,7 +7372,7 @@
         <v>PUT /v2/travelers-cheque-purchase/{tcheque-purchase-reference}</v>
       </c>
     </row>
-    <row r="54" spans="1:3">
+    <row r="54" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A54" s="45" t="s">
         <v>204</v>
       </c>
@@ -7384,7 +7384,7 @@
         <v>PUT /v2/travelers-cheque-purchase/{tcheque-purchase-reference}</v>
       </c>
     </row>
-    <row r="55" spans="1:3">
+    <row r="55" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A55" s="45" t="s">
         <v>204</v>
       </c>
@@ -7396,7 +7396,7 @@
         <v>PUT /v2/travelers-cheque-purchase/{tcheque-purchase-reference}</v>
       </c>
     </row>
-    <row r="56" spans="1:3">
+    <row r="56" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A56" s="45" t="s">
         <v>204</v>
       </c>
@@ -7408,7 +7408,7 @@
         <v>PUT /v2/travelers-cheque-purchase/{tcheque-purchase-reference}</v>
       </c>
     </row>
-    <row r="57" spans="1:3">
+    <row r="57" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A57" s="45" t="s">
         <v>204</v>
       </c>
@@ -7420,7 +7420,7 @@
         <v>PUT /v2/travelers-cheque-purchase/{tcheque-purchase-reference}</v>
       </c>
     </row>
-    <row r="58" spans="1:3">
+    <row r="58" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A58" s="45" t="s">
         <v>204</v>
       </c>
@@ -7432,7 +7432,7 @@
         <v>PUT /v2/travelers-cheque-purchase/{tcheque-purchase-reference}</v>
       </c>
     </row>
-    <row r="59" spans="1:3">
+    <row r="59" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A59" s="45" t="s">
         <v>204</v>
       </c>
@@ -7444,7 +7444,7 @@
         <v>PUT /v2/travelers-cheque-purchase/{tcheque-purchase-reference}</v>
       </c>
     </row>
-    <row r="60" spans="1:3">
+    <row r="60" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A60" s="45" t="s">
         <v>204</v>
       </c>
@@ -7456,7 +7456,7 @@
         <v>PUT /v2/travelers-cheque-purchase/{tcheque-purchase-reference}</v>
       </c>
     </row>
-    <row r="61" spans="1:3">
+    <row r="61" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A61" s="45" t="s">
         <v>204</v>
       </c>
@@ -7468,7 +7468,7 @@
         <v>PUT /v2/travelers-cheque-purchase/{tcheque-purchase-reference}</v>
       </c>
     </row>
-    <row r="62" spans="1:3">
+    <row r="62" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A62" s="45" t="s">
         <v>204</v>
       </c>
@@ -7480,7 +7480,7 @@
         <v>PUT /v2/travelers-cheque-purchase/{tcheque-purchase-reference}</v>
       </c>
     </row>
-    <row r="63" spans="1:3">
+    <row r="63" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A63" s="45" t="s">
         <v>204</v>
       </c>
@@ -7492,7 +7492,7 @@
         <v>PUT /v2/travelers-cheque-purchase/{tcheque-purchase-reference}</v>
       </c>
     </row>
-    <row r="64" spans="1:3">
+    <row r="64" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A64" s="45" t="s">
         <v>204</v>
       </c>
@@ -7504,7 +7504,7 @@
         <v>PUT /v2/travelers-cheque-purchase/{tcheque-purchase-reference}</v>
       </c>
     </row>
-    <row r="65" spans="1:3">
+    <row r="65" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A65" s="45" t="s">
         <v>204</v>
       </c>
@@ -7516,7 +7516,7 @@
         <v>PUT /v2/travelers-cheque-purchase/{tcheque-purchase-reference}</v>
       </c>
     </row>
-    <row r="66" spans="1:3">
+    <row r="66" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A66" s="45" t="s">
         <v>204</v>
       </c>
@@ -7528,7 +7528,7 @@
         <v>PUT /v2/travelers-cheque-purchase/{tcheque-purchase-reference}</v>
       </c>
     </row>
-    <row r="67" spans="1:3">
+    <row r="67" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A67" s="45" t="s">
         <v>204</v>
       </c>
@@ -7540,7 +7540,7 @@
         <v>PUT /v2/travelers-cheque-purchase/{tcheque-purchase-reference}</v>
       </c>
     </row>
-    <row r="68" spans="1:3">
+    <row r="68" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A68" s="45" t="s">
         <v>204</v>
       </c>
@@ -7552,7 +7552,7 @@
         <v>PUT /v2/travelers-cheque-purchase/{tcheque-purchase-reference}</v>
       </c>
     </row>
-    <row r="69" spans="1:3">
+    <row r="69" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A69" s="45" t="s">
         <v>204</v>
       </c>
@@ -7564,7 +7564,7 @@
         <v>PUT /v2/travelers-cheque-purchase/{tcheque-purchase-reference}</v>
       </c>
     </row>
-    <row r="70" spans="1:3">
+    <row r="70" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A70" s="45" t="s">
         <v>204</v>
       </c>
@@ -7576,7 +7576,7 @@
         <v>PUT /v2/travelers-cheque-purchase/{tcheque-purchase-reference}</v>
       </c>
     </row>
-    <row r="71" spans="1:3">
+    <row r="71" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A71" s="45" t="s">
         <v>204</v>
       </c>
@@ -7588,7 +7588,7 @@
         <v>PUT /v2/travelers-cheque-purchase/{tcheque-purchase-reference}</v>
       </c>
     </row>
-    <row r="72" spans="1:3">
+    <row r="72" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A72" s="45" t="s">
         <v>204</v>
       </c>
@@ -7600,7 +7600,7 @@
         <v>PUT /v2/travelers-cheque-purchase/{tcheque-purchase-reference}</v>
       </c>
     </row>
-    <row r="73" spans="1:3">
+    <row r="73" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A73" s="45" t="s">
         <v>204</v>
       </c>
@@ -7612,7 +7612,7 @@
         <v>PUT /v2/travelers-cheque-purchase/{tcheque-purchase-reference}</v>
       </c>
     </row>
-    <row r="74" spans="1:3">
+    <row r="74" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A74" s="45" t="s">
         <v>204</v>
       </c>
@@ -7624,7 +7624,7 @@
         <v>PUT /v2/travelers-cheque-purchase/{tcheque-purchase-reference}</v>
       </c>
     </row>
-    <row r="75" spans="1:3">
+    <row r="75" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A75" s="45" t="s">
         <v>204</v>
       </c>
@@ -7636,7 +7636,7 @@
         <v>PUT /v2/travelers-cheque-purchase/{tcheque-purchase-reference}</v>
       </c>
     </row>
-    <row r="76" spans="1:3">
+    <row r="76" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A76" s="45" t="s">
         <v>204</v>
       </c>
@@ -7648,7 +7648,7 @@
         <v>PUT /v2/travelers-cheque-purchase/{tcheque-purchase-reference}</v>
       </c>
     </row>
-    <row r="77" spans="1:3">
+    <row r="77" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A77" s="45" t="s">
         <v>204</v>
       </c>
@@ -7660,7 +7660,7 @@
         <v>PUT /v2/travelers-cheque-purchase/{tcheque-purchase-reference}</v>
       </c>
     </row>
-    <row r="78" spans="1:3">
+    <row r="78" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A78" s="45" t="s">
         <v>142</v>
       </c>
@@ -7672,7 +7672,7 @@
         <v>PATCH /v2/travelers-cheque-purchase/{tcheque-purchase-reference}</v>
       </c>
     </row>
-    <row r="79" spans="1:3">
+    <row r="79" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A79" s="45" t="s">
         <v>142</v>
       </c>
@@ -7684,7 +7684,7 @@
         <v>PATCH /v2/travelers-cheque-purchase/{tcheque-purchase-reference}</v>
       </c>
     </row>
-    <row r="80" spans="1:3">
+    <row r="80" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A80" s="45" t="s">
         <v>142</v>
       </c>
@@ -7696,7 +7696,7 @@
         <v>PATCH /v2 /vault/{request-id}/cash-request-reversal</v>
       </c>
     </row>
-    <row r="81" spans="1:3">
+    <row r="81" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A81" s="45" t="s">
         <v>142</v>
       </c>
@@ -7722,14 +7722,14 @@
       <selection activeCell="E11" sqref="E11:G11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="33.85546875" customWidth="1"/>
-    <col min="2" max="2" width="32.85546875" customWidth="1"/>
-    <col min="3" max="3" width="42.7109375" customWidth="1"/>
+    <col min="1" max="1" width="33.8984375" customWidth="1"/>
+    <col min="2" max="2" width="32.8984375" customWidth="1"/>
+    <col min="3" max="3" width="42.69921875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" s="48" t="s">
         <v>77</v>
       </c>
@@ -7740,7 +7740,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="2" spans="1:7">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" s="50" t="s">
         <v>92</v>
       </c>
@@ -7751,7 +7751,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="3" spans="1:7">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" s="50"/>
       <c r="B3" s="51">
         <v>2</v>
@@ -7760,7 +7760,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="4" spans="1:7">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" s="50"/>
       <c r="B4" s="51">
         <v>3</v>
@@ -7769,7 +7769,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="5" spans="1:7">
+    <row r="5" spans="1:7" ht="15" x14ac:dyDescent="0.35">
       <c r="A5" s="59" t="s">
         <v>95</v>
       </c>
@@ -7780,7 +7780,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="6" spans="1:7">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6" s="50"/>
       <c r="B6" s="51">
         <v>2</v>
@@ -7789,7 +7789,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="7" spans="1:7">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A7" s="50"/>
       <c r="B7" s="51">
         <v>3</v>
@@ -7798,7 +7798,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="8" spans="1:7">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A8" s="50" t="s">
         <v>99</v>
       </c>
@@ -7809,7 +7809,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="9" spans="1:7">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A9" s="50"/>
       <c r="B9" s="51">
         <v>2</v>
@@ -7818,7 +7818,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="10" spans="1:7">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A10" s="50"/>
       <c r="B10" s="51">
         <v>3</v>
@@ -7827,7 +7827,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="11" spans="1:7">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A11" s="52"/>
       <c r="B11" s="49">
         <v>4</v>
@@ -7845,7 +7845,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="12" spans="1:7">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A12" s="50" t="s">
         <v>103</v>
       </c>
@@ -7856,7 +7856,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="13" spans="1:7">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A13" s="50"/>
       <c r="B13" s="51">
         <v>2</v>
@@ -7865,7 +7865,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="14" spans="1:7">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A14" s="50"/>
       <c r="B14" s="51">
         <v>3</v>
@@ -7874,7 +7874,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="15" spans="1:7">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A15" s="50"/>
       <c r="B15" s="51">
         <v>4</v>
@@ -7883,7 +7883,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="16" spans="1:7">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A16" s="52"/>
       <c r="B16" s="51">
         <v>5</v>
@@ -7892,7 +7892,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="17" spans="1:3">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A17" s="50" t="s">
         <v>108</v>
       </c>
@@ -7903,7 +7903,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="18" spans="1:3">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A18" s="53"/>
       <c r="B18" s="54">
         <v>2</v>
@@ -7912,7 +7912,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="19" spans="1:3">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A19" s="56"/>
       <c r="B19" s="57">
         <v>3</v>
@@ -7921,7 +7921,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="20" spans="1:3">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A20" s="56" t="s">
         <v>111</v>
       </c>
@@ -7932,7 +7932,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="21" spans="1:3">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A21" s="56"/>
       <c r="B21" s="58">
         <v>2</v>
@@ -7941,12 +7941,12 @@
         <v>113</v>
       </c>
     </row>
-    <row r="22" spans="1:3">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A22" s="56"/>
       <c r="B22" s="58"/>
       <c r="C22" s="58"/>
     </row>
-    <row r="23" spans="1:3">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A23" s="60" t="s">
         <v>114</v>
       </c>
@@ -7957,7 +7957,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="24" spans="1:3">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A24" s="56"/>
       <c r="B24" s="58">
         <v>2</v>
@@ -7966,7 +7966,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="25" spans="1:3">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A25" s="56"/>
       <c r="B25" s="58">
         <v>3</v>
@@ -7975,7 +7975,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="26" spans="1:3">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A26" s="56"/>
       <c r="B26" s="58">
         <v>4</v>
@@ -7984,7 +7984,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="27" spans="1:3">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A27" s="56"/>
       <c r="B27" s="58">
         <v>5</v>
@@ -7993,19 +7993,19 @@
         <v>118</v>
       </c>
     </row>
-    <row r="28" spans="1:3">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A28" s="56"/>
       <c r="B28" s="58"/>
       <c r="C28" s="58" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="29" spans="1:3" ht="16.5" thickBot="1">
+    <row r="29" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A29" s="56"/>
       <c r="B29" s="58"/>
       <c r="C29" s="58"/>
     </row>
-    <row r="30" spans="1:3" ht="16.5" thickBot="1">
+    <row r="30" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A30" s="61" t="s">
         <v>120</v>
       </c>
@@ -8016,7 +8016,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="31" spans="1:3" ht="16.5" thickBot="1">
+    <row r="31" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A31" s="62"/>
       <c r="B31" s="58">
         <v>2</v>
@@ -8025,7 +8025,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="32" spans="1:3" ht="16.5" thickBot="1">
+    <row r="32" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A32" s="62"/>
       <c r="B32" s="58">
         <v>3</v>
@@ -8034,12 +8034,12 @@
         <v>78</v>
       </c>
     </row>
-    <row r="33" spans="1:3">
+    <row r="33" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A33" s="56"/>
       <c r="B33" s="58"/>
       <c r="C33" s="58"/>
     </row>
-    <row r="34" spans="1:3">
+    <row r="34" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A34" s="63" t="s">
         <v>123</v>
       </c>
@@ -8050,7 +8050,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="35" spans="1:3">
+    <row r="35" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A35" s="56"/>
       <c r="B35" s="58">
         <v>2</v>
@@ -8059,7 +8059,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="36" spans="1:3">
+    <row r="36" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A36" s="56"/>
       <c r="B36" s="58">
         <v>3</v>

</xml_diff>